<commit_message>
updated the q4.sql and excel
</commit_message>
<xml_diff>
--- a/Project3/Q4/Chart1.xlsx
+++ b/Project3/Q4/Chart1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/Q4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBBD5551-392B-644D-BF5F-577C849E1D2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B36130-F476-C440-B7DE-E12DE832418B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="460" windowWidth="24940" windowHeight="14580" xr2:uid="{876DCF2F-1780-CD45-AB78-84EC246CAE94}"/>
   </bookViews>
@@ -16,11 +16,15 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$1:$A$9</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$1:$B$9</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Feuil1!$A$1:$A$9</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Feuil1!$B$1:$B$9</definedName>
-    <definedName name="Sales" localSheetId="0">Feuil1!$A$1:$B$9</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$B$1:$B$12</definedName>
+    <definedName name="Sales" localSheetId="0">Feuil1!#REF!</definedName>
+    <definedName name="Sales_1" localSheetId="0">Feuil1!$A$1:$B$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,8 +37,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{C1ADD4D2-A8E8-3E4E-ABB8-5175CFFD4914}" name="Sales" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/Sales.csv" thousands=" " comma="1">
+  <connection id="1" xr16:uid="{9C745A3B-C6A3-1D4E-B913-2112B062ED3E}" name="Sales1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/Q4/Sales.csv" thousands=" " comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -101,10 +105,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -176,85 +180,58 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
-            <a:ln>
+            <a:ln w="25400">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Feuil1!$A$1:$A$9</c:f>
+              <c:f>Feuil1!$B$1:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Feuil1!$B$1:$B$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -262,7 +239,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-53F3-9A4C-AF03-E8AC1E5DE3DE}"/>
+              <c16:uniqueId val="{00000000-E466-A148-95EB-8A6EFD707BAF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -275,7 +252,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="61302047"/>
         <c:axId val="61303743"/>
       </c:barChart>
@@ -552,42 +528,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1136,7 +1078,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sales" connectionId="1" xr16:uid="{D8F87E73-CF7B-5542-985F-54309D6E687D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sales_1" connectionId="1" xr16:uid="{E0EA6D63-A335-AC44-AE12-A9A6F68A4D23}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1436,16 +1378,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9E5E62-F40D-384C-A46C-39B5FDEC5C2F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1458,65 +1402,89 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>4</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>1</v>
       </c>
     </row>

</xml_diff>